<commit_message>
fixed permutation importance stuff
</commit_message>
<xml_diff>
--- a/planB/data/rf_out/RF_important_features.xlsx
+++ b/planB/data/rf_out/RF_important_features.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jake/Desktop/DSS_repo/BTCMiningCO2Footprint/planB/data/rf_out/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8565C86-1E78-4E4A-A8CB-2B619D22467F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85B6D506-6CA1-C042-A56B-2FC21A2CCDB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="36420" yWindow="500" windowWidth="27640" windowHeight="16940" xr2:uid="{CB2A7D81-577F-B948-B7BD-8F247062CBE1}"/>
+    <workbookView xWindow="1360" yWindow="500" windowWidth="30540" windowHeight="19120" xr2:uid="{CB2A7D81-577F-B948-B7BD-8F247062CBE1}"/>
   </bookViews>
   <sheets>
     <sheet name="by method" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2541" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2694" uniqueCount="94">
   <si>
     <t>1: Both Urban and Rural, All Income</t>
   </si>
@@ -340,12 +340,54 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFDECCFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC1C6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="9">
@@ -448,7 +490,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -467,8 +509,16 @@
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -476,8 +526,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -487,27 +538,38 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFFC1C6"/>
+      <color rgb="FFDECCFF"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -818,18 +880,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F670D600-BE7B-A546-8B6E-27B91BA76A6F}">
   <dimension ref="B1:AM82"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+    <sheetView tabSelected="1" topLeftCell="S1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="0.83203125" customWidth="1"/>
+    <col min="2" max="2" width="12.6640625" customWidth="1"/>
     <col min="3" max="3" width="9" customWidth="1"/>
+    <col min="4" max="4" width="12.83203125" customWidth="1"/>
     <col min="5" max="5" width="9" customWidth="1"/>
+    <col min="6" max="6" width="12.83203125" customWidth="1"/>
     <col min="7" max="7" width="9" customWidth="1"/>
+    <col min="8" max="8" width="12.6640625" customWidth="1"/>
     <col min="9" max="9" width="9" customWidth="1"/>
+    <col min="10" max="10" width="12.5" customWidth="1"/>
     <col min="11" max="11" width="9" customWidth="1"/>
+    <col min="12" max="12" width="12.5" customWidth="1"/>
     <col min="13" max="13" width="9" customWidth="1"/>
     <col min="14" max="14" width="3.33203125" customWidth="1"/>
     <col min="16" max="16" width="9" customWidth="1"/>
@@ -839,163 +907,169 @@
     <col min="24" max="24" width="9" customWidth="1"/>
     <col min="26" max="26" width="9" customWidth="1"/>
     <col min="27" max="27" width="3.33203125" customWidth="1"/>
+    <col min="28" max="28" width="12.6640625" customWidth="1"/>
+    <col min="30" max="30" width="12.33203125" customWidth="1"/>
+    <col min="32" max="32" width="12.5" customWidth="1"/>
     <col min="33" max="33" width="9" customWidth="1"/>
+    <col min="34" max="34" width="12.1640625" customWidth="1"/>
     <col min="35" max="35" width="9" customWidth="1"/>
+    <col min="36" max="36" width="12.5" customWidth="1"/>
     <col min="37" max="37" width="9" customWidth="1"/>
+    <col min="38" max="38" width="12.5" customWidth="1"/>
     <col min="39" max="39" width="9" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:39" ht="5" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="2" spans="2:39" x14ac:dyDescent="0.2">
-      <c r="B2" s="20" t="s">
+      <c r="B2" s="14" t="s">
         <v>89</v>
       </c>
-      <c r="C2" s="21"/>
-      <c r="D2" s="21"/>
-      <c r="E2" s="21"/>
-      <c r="F2" s="21"/>
-      <c r="G2" s="21"/>
-      <c r="H2" s="21"/>
-      <c r="I2" s="21"/>
-      <c r="J2" s="21"/>
-      <c r="K2" s="21"/>
-      <c r="L2" s="21"/>
-      <c r="M2" s="22"/>
-      <c r="O2" s="20" t="s">
+      <c r="C2" s="15"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="15"/>
+      <c r="F2" s="15"/>
+      <c r="G2" s="15"/>
+      <c r="H2" s="15"/>
+      <c r="I2" s="15"/>
+      <c r="J2" s="15"/>
+      <c r="K2" s="15"/>
+      <c r="L2" s="15"/>
+      <c r="M2" s="16"/>
+      <c r="O2" s="14" t="s">
         <v>90</v>
       </c>
-      <c r="P2" s="21"/>
-      <c r="Q2" s="21"/>
-      <c r="R2" s="21"/>
-      <c r="S2" s="21"/>
-      <c r="T2" s="21"/>
-      <c r="U2" s="21"/>
-      <c r="V2" s="21"/>
-      <c r="W2" s="21"/>
-      <c r="X2" s="21"/>
-      <c r="Y2" s="21"/>
-      <c r="Z2" s="22"/>
-      <c r="AB2" s="20" t="s">
+      <c r="P2" s="15"/>
+      <c r="Q2" s="15"/>
+      <c r="R2" s="15"/>
+      <c r="S2" s="15"/>
+      <c r="T2" s="15"/>
+      <c r="U2" s="15"/>
+      <c r="V2" s="15"/>
+      <c r="W2" s="15"/>
+      <c r="X2" s="15"/>
+      <c r="Y2" s="15"/>
+      <c r="Z2" s="16"/>
+      <c r="AB2" s="14" t="s">
         <v>91</v>
       </c>
-      <c r="AC2" s="21"/>
-      <c r="AD2" s="21"/>
-      <c r="AE2" s="21"/>
-      <c r="AF2" s="21"/>
-      <c r="AG2" s="21"/>
-      <c r="AH2" s="21"/>
-      <c r="AI2" s="21"/>
-      <c r="AJ2" s="21"/>
-      <c r="AK2" s="21"/>
-      <c r="AL2" s="21"/>
-      <c r="AM2" s="22"/>
+      <c r="AC2" s="15"/>
+      <c r="AD2" s="15"/>
+      <c r="AE2" s="15"/>
+      <c r="AF2" s="15"/>
+      <c r="AG2" s="15"/>
+      <c r="AH2" s="15"/>
+      <c r="AI2" s="15"/>
+      <c r="AJ2" s="15"/>
+      <c r="AK2" s="15"/>
+      <c r="AL2" s="15"/>
+      <c r="AM2" s="16"/>
     </row>
     <row r="3" spans="2:39" x14ac:dyDescent="0.2">
-      <c r="B3" s="20" t="s">
+      <c r="B3" s="14" t="s">
         <v>92</v>
       </c>
-      <c r="C3" s="21"/>
-      <c r="D3" s="21" t="s">
+      <c r="C3" s="15"/>
+      <c r="D3" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="E3" s="21"/>
-      <c r="F3" s="21" t="s">
+      <c r="E3" s="15"/>
+      <c r="F3" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="G3" s="21"/>
-      <c r="H3" s="21" t="s">
+      <c r="G3" s="15"/>
+      <c r="H3" s="15" t="s">
         <v>93</v>
       </c>
-      <c r="I3" s="21"/>
-      <c r="J3" s="21" t="s">
+      <c r="I3" s="15"/>
+      <c r="J3" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="K3" s="21"/>
-      <c r="L3" s="21" t="s">
+      <c r="K3" s="15"/>
+      <c r="L3" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="M3" s="22"/>
-      <c r="O3" s="20" t="s">
+      <c r="M3" s="16"/>
+      <c r="O3" s="14" t="s">
         <v>92</v>
       </c>
-      <c r="P3" s="21"/>
-      <c r="Q3" s="21" t="s">
+      <c r="P3" s="15"/>
+      <c r="Q3" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="R3" s="21"/>
-      <c r="S3" s="21" t="s">
+      <c r="R3" s="15"/>
+      <c r="S3" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="T3" s="21"/>
-      <c r="U3" s="21" t="s">
+      <c r="T3" s="15"/>
+      <c r="U3" s="15" t="s">
         <v>93</v>
       </c>
-      <c r="V3" s="21"/>
-      <c r="W3" s="21" t="s">
+      <c r="V3" s="15"/>
+      <c r="W3" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="X3" s="21"/>
-      <c r="Y3" s="21" t="s">
+      <c r="X3" s="15"/>
+      <c r="Y3" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="Z3" s="22"/>
-      <c r="AB3" s="20" t="s">
+      <c r="Z3" s="16"/>
+      <c r="AB3" s="14" t="s">
         <v>92</v>
       </c>
-      <c r="AC3" s="21"/>
-      <c r="AD3" s="21" t="s">
+      <c r="AC3" s="15"/>
+      <c r="AD3" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="AE3" s="21"/>
-      <c r="AF3" s="21" t="s">
+      <c r="AE3" s="15"/>
+      <c r="AF3" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="AG3" s="21"/>
-      <c r="AH3" s="21" t="s">
+      <c r="AG3" s="15"/>
+      <c r="AH3" s="15" t="s">
         <v>93</v>
       </c>
-      <c r="AI3" s="21"/>
-      <c r="AJ3" s="21" t="s">
+      <c r="AI3" s="15"/>
+      <c r="AJ3" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="AK3" s="21"/>
-      <c r="AL3" s="21" t="s">
+      <c r="AK3" s="15"/>
+      <c r="AL3" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="AM3" s="22"/>
+      <c r="AM3" s="16"/>
     </row>
     <row r="4" spans="2:39" x14ac:dyDescent="0.2">
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="23" t="s">
         <v>9</v>
       </c>
       <c r="C4" s="7">
         <v>0.16047042666438899</v>
       </c>
-      <c r="D4" s="7" t="s">
+      <c r="D4" s="24" t="s">
         <v>9</v>
       </c>
       <c r="E4" s="7">
         <v>0.16658057025509901</v>
       </c>
-      <c r="F4" s="7" t="s">
+      <c r="F4" s="26" t="s">
         <v>10</v>
       </c>
       <c r="G4" s="7">
         <v>0.123435216919571</v>
       </c>
-      <c r="H4" s="7" t="s">
+      <c r="H4" s="24" t="s">
         <v>9</v>
       </c>
       <c r="I4" s="7">
         <v>0.14134313275666499</v>
       </c>
-      <c r="J4" s="7" t="s">
+      <c r="J4" s="24" t="s">
         <v>9</v>
       </c>
       <c r="K4" s="7">
         <v>0.14265107861162801</v>
       </c>
-      <c r="L4" s="7" t="s">
+      <c r="L4" s="24" t="s">
         <v>9</v>
       </c>
       <c r="M4" s="5">
@@ -1037,37 +1111,37 @@
       <c r="Z4" s="5">
         <v>7.0831389934541203E-2</v>
       </c>
-      <c r="AB4" s="23" t="s">
-        <v>88</v>
-      </c>
-      <c r="AC4" s="24" t="s">
-        <v>88</v>
-      </c>
-      <c r="AD4" s="24" t="s">
-        <v>88</v>
-      </c>
-      <c r="AE4" s="24" t="s">
-        <v>88</v>
-      </c>
-      <c r="AF4" s="7" t="s">
+      <c r="AB4" s="36" t="s">
+        <v>11</v>
+      </c>
+      <c r="AC4">
+        <v>1.7897645281229901E-2</v>
+      </c>
+      <c r="AD4" s="36" t="s">
+        <v>11</v>
+      </c>
+      <c r="AE4">
+        <v>1.7390847296468202E-2</v>
+      </c>
+      <c r="AF4" s="28" t="s">
         <v>11</v>
       </c>
       <c r="AG4" s="7">
         <v>1.46022081575671E-2</v>
       </c>
-      <c r="AH4" s="7" t="s">
+      <c r="AH4" s="28" t="s">
         <v>11</v>
       </c>
       <c r="AI4" s="7">
         <v>3.2653301315025397E-2</v>
       </c>
-      <c r="AJ4" s="7" t="s">
+      <c r="AJ4" s="28" t="s">
         <v>11</v>
       </c>
       <c r="AK4" s="7">
         <v>2.861667371522E-2</v>
       </c>
-      <c r="AL4" s="7" t="s">
+      <c r="AL4" s="26" t="s">
         <v>10</v>
       </c>
       <c r="AM4" s="5">
@@ -1075,37 +1149,37 @@
       </c>
     </row>
     <row r="5" spans="2:39" x14ac:dyDescent="0.2">
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="25" t="s">
         <v>10</v>
       </c>
       <c r="C5" s="7">
         <v>9.6357395716446095E-2</v>
       </c>
-      <c r="D5" s="7" t="s">
+      <c r="D5" s="26" t="s">
         <v>10</v>
       </c>
       <c r="E5" s="7">
         <v>0.101112122353365</v>
       </c>
-      <c r="F5" s="7" t="s">
+      <c r="F5" s="24" t="s">
         <v>9</v>
       </c>
       <c r="G5" s="7">
         <v>0.117946382373509</v>
       </c>
-      <c r="H5" s="7" t="s">
+      <c r="H5" s="26" t="s">
         <v>10</v>
       </c>
       <c r="I5" s="7">
         <v>0.109953559830305</v>
       </c>
-      <c r="J5" s="7" t="s">
+      <c r="J5" s="26" t="s">
         <v>10</v>
       </c>
       <c r="K5" s="7">
         <v>0.11126430571450401</v>
       </c>
-      <c r="L5" s="7" t="s">
+      <c r="L5" s="26" t="s">
         <v>10</v>
       </c>
       <c r="M5" s="5">
@@ -1147,29 +1221,37 @@
       <c r="Z5" s="5">
         <v>5.5345630725479197E-2</v>
       </c>
-      <c r="AB5" s="2"/>
-      <c r="AC5" s="7"/>
-      <c r="AD5" s="7"/>
-      <c r="AE5" s="7"/>
-      <c r="AF5" s="7" t="s">
+      <c r="AB5" s="35" t="s">
+        <v>10</v>
+      </c>
+      <c r="AC5">
+        <v>9.8341210630012808E-3</v>
+      </c>
+      <c r="AD5" s="35" t="s">
+        <v>10</v>
+      </c>
+      <c r="AE5">
+        <v>8.7964257248314397E-3</v>
+      </c>
+      <c r="AF5" s="40" t="s">
         <v>32</v>
       </c>
       <c r="AG5" s="7">
         <v>8.8752213791343793E-3</v>
       </c>
-      <c r="AH5" s="7" t="s">
+      <c r="AH5" s="32" t="s">
         <v>13</v>
       </c>
       <c r="AI5" s="7">
         <v>2.0126790100643398E-2</v>
       </c>
-      <c r="AJ5" s="7" t="s">
+      <c r="AJ5" s="32" t="s">
         <v>13</v>
       </c>
       <c r="AK5" s="7">
         <v>2.6911680204498099E-2</v>
       </c>
-      <c r="AL5" s="7" t="s">
+      <c r="AL5" s="28" t="s">
         <v>11</v>
       </c>
       <c r="AM5" s="5">
@@ -1177,37 +1259,37 @@
       </c>
     </row>
     <row r="6" spans="2:39" x14ac:dyDescent="0.2">
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="27" t="s">
         <v>11</v>
       </c>
       <c r="C6" s="7">
         <v>4.0532795190764401E-2</v>
       </c>
-      <c r="D6" s="7" t="s">
+      <c r="D6" s="28" t="s">
         <v>11</v>
       </c>
       <c r="E6" s="7">
         <v>4.0495174244186201E-2</v>
       </c>
-      <c r="F6" s="7" t="s">
+      <c r="F6" s="29" t="s">
         <v>12</v>
       </c>
       <c r="G6" s="7">
         <v>4.5328762400968003E-2</v>
       </c>
-      <c r="H6" s="7" t="s">
+      <c r="H6" s="28" t="s">
         <v>11</v>
       </c>
       <c r="I6" s="7">
         <v>4.6847004255811703E-2</v>
       </c>
-      <c r="J6" s="7" t="s">
+      <c r="J6" s="28" t="s">
         <v>11</v>
       </c>
       <c r="K6" s="7">
         <v>4.24939000317743E-2</v>
       </c>
-      <c r="L6" s="7" t="s">
+      <c r="L6" s="28" t="s">
         <v>11</v>
       </c>
       <c r="M6" s="5">
@@ -1249,23 +1331,31 @@
       <c r="Z6" s="5">
         <v>5.47459714817475E-2</v>
       </c>
-      <c r="AB6" s="2"/>
-      <c r="AC6" s="7"/>
-      <c r="AD6" s="7"/>
-      <c r="AE6" s="7"/>
-      <c r="AF6" s="7" t="s">
+      <c r="AB6" s="39" t="s">
+        <v>32</v>
+      </c>
+      <c r="AC6">
+        <v>7.9615442652960396E-3</v>
+      </c>
+      <c r="AD6" s="41" t="s">
+        <v>29</v>
+      </c>
+      <c r="AE6">
+        <v>7.1996980375613299E-3</v>
+      </c>
+      <c r="AF6" s="24" t="s">
         <v>9</v>
       </c>
       <c r="AG6" s="7">
         <v>7.1950757112848197E-3</v>
       </c>
-      <c r="AH6" s="7" t="s">
+      <c r="AH6" s="42" t="s">
         <v>29</v>
       </c>
       <c r="AI6" s="7">
         <v>1.38540385505254E-2</v>
       </c>
-      <c r="AJ6" s="7" t="s">
+      <c r="AJ6" s="24" t="s">
         <v>9</v>
       </c>
       <c r="AK6" s="7">
@@ -1279,31 +1369,31 @@
       </c>
     </row>
     <row r="7" spans="2:39" x14ac:dyDescent="0.2">
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="30" t="s">
         <v>12</v>
       </c>
       <c r="C7" s="7">
         <v>3.1630122621181797E-2</v>
       </c>
-      <c r="D7" s="7" t="s">
+      <c r="D7" s="32" t="s">
         <v>13</v>
       </c>
       <c r="E7" s="7">
         <v>3.4885072734609897E-2</v>
       </c>
-      <c r="F7" s="7" t="s">
+      <c r="F7" s="28" t="s">
         <v>11</v>
       </c>
       <c r="G7" s="7">
         <v>4.4058424468310903E-2</v>
       </c>
-      <c r="H7" s="7" t="s">
+      <c r="H7" s="32" t="s">
         <v>13</v>
       </c>
       <c r="I7" s="7">
         <v>3.0201232740022298E-2</v>
       </c>
-      <c r="J7" s="7" t="s">
+      <c r="J7" s="32" t="s">
         <v>13</v>
       </c>
       <c r="K7" s="7">
@@ -1351,29 +1441,37 @@
       <c r="Z7" s="5">
         <v>3.8072738161771098E-2</v>
       </c>
-      <c r="AB7" s="2"/>
-      <c r="AC7" s="7"/>
-      <c r="AD7" s="7"/>
-      <c r="AE7" s="7"/>
-      <c r="AF7" s="7" t="s">
+      <c r="AB7" s="41" t="s">
+        <v>29</v>
+      </c>
+      <c r="AC7">
+        <v>5.9676784478187002E-3</v>
+      </c>
+      <c r="AD7" s="34" t="s">
+        <v>9</v>
+      </c>
+      <c r="AE7">
+        <v>5.2790614405028103E-3</v>
+      </c>
+      <c r="AF7" s="26" t="s">
         <v>10</v>
       </c>
       <c r="AG7" s="7">
         <v>6.1030391854946502E-3</v>
       </c>
-      <c r="AH7" s="7" t="s">
+      <c r="AH7" s="40" t="s">
         <v>46</v>
       </c>
       <c r="AI7" s="7">
         <v>1.2704296845491399E-2</v>
       </c>
-      <c r="AJ7" s="7" t="s">
+      <c r="AJ7" s="42" t="s">
         <v>29</v>
       </c>
       <c r="AK7" s="7">
         <v>1.13215535191853E-2</v>
       </c>
-      <c r="AL7" s="7" t="s">
+      <c r="AL7" s="24" t="s">
         <v>9</v>
       </c>
       <c r="AM7" s="5">
@@ -1381,13 +1479,13 @@
       </c>
     </row>
     <row r="8" spans="2:39" x14ac:dyDescent="0.2">
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="31" t="s">
         <v>13</v>
       </c>
       <c r="C8" s="7">
         <v>2.8411121713496201E-2</v>
       </c>
-      <c r="D8" s="7" t="s">
+      <c r="D8" s="29" t="s">
         <v>12</v>
       </c>
       <c r="E8" s="7">
@@ -1399,19 +1497,19 @@
       <c r="G8" s="7">
         <v>2.8651031186155598E-2</v>
       </c>
-      <c r="H8" s="7" t="s">
+      <c r="H8" s="29" t="s">
         <v>12</v>
       </c>
       <c r="I8" s="7">
         <v>2.6628775514551999E-2</v>
       </c>
-      <c r="J8" s="7" t="s">
+      <c r="J8" s="29" t="s">
         <v>12</v>
       </c>
       <c r="K8" s="7">
         <v>2.5643529146983798E-2</v>
       </c>
-      <c r="L8" s="7" t="s">
+      <c r="L8" s="32" t="s">
         <v>13</v>
       </c>
       <c r="M8" s="5">
@@ -1453,23 +1551,31 @@
       <c r="Z8" s="5">
         <v>3.2190288916356898E-2</v>
       </c>
-      <c r="AB8" s="2"/>
-      <c r="AC8" s="7"/>
-      <c r="AD8" s="7"/>
-      <c r="AE8" s="7"/>
+      <c r="AB8" s="34" t="s">
+        <v>9</v>
+      </c>
+      <c r="AC8">
+        <v>5.2676469892237402E-3</v>
+      </c>
+      <c r="AD8" s="37" t="s">
+        <v>12</v>
+      </c>
+      <c r="AE8">
+        <v>3.9949972611768598E-3</v>
+      </c>
       <c r="AF8" s="7" t="s">
         <v>63</v>
       </c>
       <c r="AG8" s="7">
         <v>5.3900012672668798E-3</v>
       </c>
-      <c r="AH8" s="7" t="s">
+      <c r="AH8" s="24" t="s">
         <v>9</v>
       </c>
       <c r="AI8" s="7">
         <v>1.1363273271393901E-2</v>
       </c>
-      <c r="AJ8" s="7" t="s">
+      <c r="AJ8" s="26" t="s">
         <v>10</v>
       </c>
       <c r="AK8" s="7">
@@ -1492,10 +1598,10 @@
       <c r="D9" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="E9" s="7">
+      <c r="E9" s="33">
         <v>2.64509295211021E-2</v>
       </c>
-      <c r="F9" s="7" t="s">
+      <c r="F9" s="32" t="s">
         <v>13</v>
       </c>
       <c r="G9" s="7">
@@ -1555,23 +1661,31 @@
       <c r="Z9" s="5">
         <v>2.97542072675837E-2</v>
       </c>
-      <c r="AB9" s="2"/>
-      <c r="AC9" s="7"/>
-      <c r="AD9" s="7"/>
-      <c r="AE9" s="7"/>
+      <c r="AB9" t="s">
+        <v>18</v>
+      </c>
+      <c r="AC9">
+        <v>3.6556136824557198E-3</v>
+      </c>
+      <c r="AD9" t="s">
+        <v>18</v>
+      </c>
+      <c r="AE9">
+        <v>3.7853648757950002E-3</v>
+      </c>
       <c r="AF9" s="7" t="s">
         <v>38</v>
       </c>
       <c r="AG9" s="7">
         <v>4.2876261200726499E-3</v>
       </c>
-      <c r="AH9" s="7" t="s">
+      <c r="AH9" s="26" t="s">
         <v>10</v>
       </c>
       <c r="AI9" s="7">
         <v>9.9007783255706493E-3</v>
       </c>
-      <c r="AJ9" s="7" t="s">
+      <c r="AJ9" s="29" t="s">
         <v>12</v>
       </c>
       <c r="AK9" s="7">
@@ -1657,10 +1771,18 @@
       <c r="Z10" s="5">
         <v>2.5865466269533701E-2</v>
       </c>
-      <c r="AB10" s="2"/>
-      <c r="AC10" s="7"/>
-      <c r="AD10" s="7"/>
-      <c r="AE10" s="7"/>
+      <c r="AB10" s="38" t="s">
+        <v>13</v>
+      </c>
+      <c r="AC10">
+        <v>2.93400292301388E-3</v>
+      </c>
+      <c r="AD10" s="38" t="s">
+        <v>13</v>
+      </c>
+      <c r="AE10">
+        <v>3.4158392375531498E-3</v>
+      </c>
       <c r="AF10" s="7" t="s">
         <v>16</v>
       </c>
@@ -1759,17 +1881,25 @@
       <c r="Z11" s="5">
         <v>2.4770372318713801E-2</v>
       </c>
-      <c r="AB11" s="2"/>
-      <c r="AC11" s="7"/>
-      <c r="AD11" s="7"/>
-      <c r="AE11" s="7"/>
+      <c r="AB11" t="s">
+        <v>34</v>
+      </c>
+      <c r="AC11">
+        <v>2.88682538706647E-3</v>
+      </c>
+      <c r="AD11" t="s">
+        <v>33</v>
+      </c>
+      <c r="AE11">
+        <v>3.2735900888736999E-3</v>
+      </c>
       <c r="AF11" s="7" t="s">
         <v>18</v>
       </c>
       <c r="AG11" s="7">
         <v>3.1342873760778702E-3</v>
       </c>
-      <c r="AH11" s="7" t="s">
+      <c r="AH11" s="29" t="s">
         <v>12</v>
       </c>
       <c r="AI11" s="7">
@@ -1861,10 +1991,18 @@
       <c r="Z12" s="5">
         <v>2.069137091921E-2</v>
       </c>
-      <c r="AB12" s="2"/>
-      <c r="AC12" s="7"/>
-      <c r="AD12" s="7"/>
-      <c r="AE12" s="7"/>
+      <c r="AB12" t="s">
+        <v>16</v>
+      </c>
+      <c r="AC12">
+        <v>2.65465893397502E-3</v>
+      </c>
+      <c r="AD12" s="39" t="s">
+        <v>32</v>
+      </c>
+      <c r="AE12">
+        <v>3.1020087802926099E-3</v>
+      </c>
       <c r="AF12" s="7" t="s">
         <v>45</v>
       </c>
@@ -1877,7 +2015,7 @@
       <c r="AI12" s="7">
         <v>8.1259678577831999E-3</v>
       </c>
-      <c r="AJ12" s="7" t="s">
+      <c r="AJ12" s="40" t="s">
         <v>46</v>
       </c>
       <c r="AK12" s="7">
@@ -1963,10 +2101,18 @@
       <c r="Z13" s="5">
         <v>1.7676447326875799E-2</v>
       </c>
-      <c r="AB13" s="2"/>
-      <c r="AC13" s="7"/>
-      <c r="AD13" s="7"/>
-      <c r="AE13" s="7"/>
+      <c r="AB13" t="s">
+        <v>38</v>
+      </c>
+      <c r="AC13">
+        <v>2.64732012132272E-3</v>
+      </c>
+      <c r="AD13" t="s">
+        <v>16</v>
+      </c>
+      <c r="AE13">
+        <v>2.7479972800709298E-3</v>
+      </c>
       <c r="AF13" s="7" t="s">
         <v>34</v>
       </c>
@@ -1985,7 +2131,7 @@
       <c r="AK13" s="7">
         <v>6.3775759451482001E-3</v>
       </c>
-      <c r="AL13" s="7" t="s">
+      <c r="AL13" s="29" t="s">
         <v>12</v>
       </c>
       <c r="AM13" s="5">
@@ -2065,10 +2211,18 @@
       <c r="Z14" s="5">
         <v>1.2072386078192001E-2</v>
       </c>
-      <c r="AB14" s="2"/>
-      <c r="AC14" s="7"/>
-      <c r="AD14" s="7"/>
-      <c r="AE14" s="7"/>
+      <c r="AB14" s="37" t="s">
+        <v>12</v>
+      </c>
+      <c r="AC14">
+        <v>2.5337048033906399E-3</v>
+      </c>
+      <c r="AD14" t="s">
+        <v>34</v>
+      </c>
+      <c r="AE14">
+        <v>2.5601415577881301E-3</v>
+      </c>
       <c r="AF14" s="7" t="s">
         <v>65</v>
       </c>
@@ -2167,10 +2321,18 @@
       <c r="Z15" s="5">
         <v>1.18801274078755E-2</v>
       </c>
-      <c r="AB15" s="2"/>
-      <c r="AC15" s="7"/>
-      <c r="AD15" s="7"/>
-      <c r="AE15" s="7"/>
+      <c r="AB15" t="s">
+        <v>28</v>
+      </c>
+      <c r="AC15">
+        <v>2.4451504732970202E-3</v>
+      </c>
+      <c r="AD15" t="s">
+        <v>38</v>
+      </c>
+      <c r="AE15">
+        <v>2.3503150276109599E-3</v>
+      </c>
       <c r="AF15" s="7" t="s">
         <v>62</v>
       </c>
@@ -2189,7 +2351,7 @@
       <c r="AK15" s="7">
         <v>6.0879413830952998E-3</v>
       </c>
-      <c r="AL15" s="7" t="s">
+      <c r="AL15" s="32" t="s">
         <v>13</v>
       </c>
       <c r="AM15" s="5">
@@ -2269,10 +2431,18 @@
       <c r="Z16" s="5">
         <v>1.05026474958044E-2</v>
       </c>
-      <c r="AB16" s="2"/>
-      <c r="AC16" s="7"/>
-      <c r="AD16" s="7"/>
-      <c r="AE16" s="7"/>
+      <c r="AB16" t="s">
+        <v>21</v>
+      </c>
+      <c r="AC16">
+        <v>2.4358205146186199E-3</v>
+      </c>
+      <c r="AD16" t="s">
+        <v>28</v>
+      </c>
+      <c r="AE16">
+        <v>2.3426494579206199E-3</v>
+      </c>
       <c r="AF16" s="7" t="s">
         <v>20</v>
       </c>
@@ -2371,10 +2541,18 @@
       <c r="Z17" s="5">
         <v>9.1086752994097003E-3</v>
       </c>
-      <c r="AB17" s="2"/>
-      <c r="AC17" s="7"/>
-      <c r="AD17" s="7"/>
-      <c r="AE17" s="7"/>
+      <c r="AB17" t="s">
+        <v>27</v>
+      </c>
+      <c r="AC17">
+        <v>2.3033841347155398E-3</v>
+      </c>
+      <c r="AD17" t="s">
+        <v>21</v>
+      </c>
+      <c r="AE17">
+        <v>2.32228370222619E-3</v>
+      </c>
       <c r="AF17" s="7" t="s">
         <v>39</v>
       </c>
@@ -2473,10 +2651,18 @@
       <c r="Z18" s="5">
         <v>8.5352844237140506E-3</v>
       </c>
-      <c r="AB18" s="2"/>
-      <c r="AC18" s="7"/>
-      <c r="AD18" s="7"/>
-      <c r="AE18" s="7"/>
+      <c r="AB18" t="s">
+        <v>33</v>
+      </c>
+      <c r="AC18">
+        <v>2.2311655434846698E-3</v>
+      </c>
+      <c r="AD18" t="s">
+        <v>23</v>
+      </c>
+      <c r="AE18">
+        <v>1.6934405787107699E-3</v>
+      </c>
       <c r="AF18" s="7" t="s">
         <v>52</v>
       </c>
@@ -2575,10 +2761,18 @@
       <c r="Z19" s="5">
         <v>6.1407934908061096E-3</v>
       </c>
-      <c r="AB19" s="2"/>
-      <c r="AC19" s="7"/>
-      <c r="AD19" s="7"/>
-      <c r="AE19" s="7"/>
+      <c r="AB19" t="s">
+        <v>23</v>
+      </c>
+      <c r="AC19">
+        <v>1.88328177799344E-3</v>
+      </c>
+      <c r="AD19" t="s">
+        <v>31</v>
+      </c>
+      <c r="AE19">
+        <v>1.5051628370864099E-3</v>
+      </c>
       <c r="AF19" s="7" t="s">
         <v>28</v>
       </c>
@@ -2677,10 +2871,18 @@
       <c r="Z20" s="5">
         <v>5.8454820543656803E-3</v>
       </c>
-      <c r="AB20" s="2"/>
-      <c r="AC20" s="7"/>
-      <c r="AD20" s="7"/>
-      <c r="AE20" s="7"/>
+      <c r="AB20" t="s">
+        <v>22</v>
+      </c>
+      <c r="AC20">
+        <v>1.82500179609053E-3</v>
+      </c>
+      <c r="AD20" t="s">
+        <v>24</v>
+      </c>
+      <c r="AE20">
+        <v>1.4758521833334599E-3</v>
+      </c>
       <c r="AF20" s="7" t="s">
         <v>30</v>
       </c>
@@ -2779,11 +2981,19 @@
       <c r="Z21" s="5">
         <v>3.5010297795902302E-3</v>
       </c>
-      <c r="AB21" s="2"/>
-      <c r="AC21" s="7"/>
-      <c r="AD21" s="7"/>
-      <c r="AE21" s="7"/>
-      <c r="AF21" s="7" t="s">
+      <c r="AB21" t="s">
+        <v>37</v>
+      </c>
+      <c r="AC21">
+        <v>1.7023341684190201E-3</v>
+      </c>
+      <c r="AD21" t="s">
+        <v>30</v>
+      </c>
+      <c r="AE21">
+        <v>1.3860653598055299E-3</v>
+      </c>
+      <c r="AF21" s="29" t="s">
         <v>12</v>
       </c>
       <c r="AG21" s="7">
@@ -2881,10 +3091,18 @@
       <c r="Z22" s="5">
         <v>3.1524900470035E-3</v>
       </c>
-      <c r="AB22" s="2"/>
-      <c r="AC22" s="7"/>
-      <c r="AD22" s="7"/>
-      <c r="AE22" s="7"/>
+      <c r="AB22" t="s">
+        <v>26</v>
+      </c>
+      <c r="AC22">
+        <v>1.63740886903635E-3</v>
+      </c>
+      <c r="AD22" t="s">
+        <v>43</v>
+      </c>
+      <c r="AE22">
+        <v>1.35141435378784E-3</v>
+      </c>
       <c r="AF22" s="7" t="s">
         <v>64</v>
       </c>
@@ -2983,10 +3201,18 @@
       <c r="Z23" s="5">
         <v>3.0162869467675402E-3</v>
       </c>
-      <c r="AB23" s="2"/>
-      <c r="AC23" s="7"/>
-      <c r="AD23" s="7"/>
-      <c r="AE23" s="7"/>
+      <c r="AB23" t="s">
+        <v>45</v>
+      </c>
+      <c r="AC23">
+        <v>1.54660947478961E-3</v>
+      </c>
+      <c r="AD23" t="s">
+        <v>50</v>
+      </c>
+      <c r="AE23">
+        <v>1.29631582342876E-3</v>
+      </c>
       <c r="AF23" s="7" t="s">
         <v>22</v>
       </c>
@@ -3085,10 +3311,18 @@
       <c r="Z24" s="5">
         <v>2.0126166376073602E-3</v>
       </c>
-      <c r="AB24" s="2"/>
-      <c r="AC24" s="7"/>
-      <c r="AD24" s="7"/>
-      <c r="AE24" s="7"/>
+      <c r="AB24" t="s">
+        <v>20</v>
+      </c>
+      <c r="AC24">
+        <v>1.51246856592631E-3</v>
+      </c>
+      <c r="AD24" t="s">
+        <v>42</v>
+      </c>
+      <c r="AE24">
+        <v>1.29392620836403E-3</v>
+      </c>
       <c r="AF24" s="7" t="s">
         <v>25</v>
       </c>
@@ -3187,10 +3421,18 @@
       <c r="Z25" s="5">
         <v>1.46262643165191E-3</v>
       </c>
-      <c r="AB25" s="2"/>
-      <c r="AC25" s="7"/>
-      <c r="AD25" s="7"/>
-      <c r="AE25" s="7"/>
+      <c r="AB25" t="s">
+        <v>39</v>
+      </c>
+      <c r="AC25">
+        <v>1.47850643198429E-3</v>
+      </c>
+      <c r="AD25" t="s">
+        <v>19</v>
+      </c>
+      <c r="AE25">
+        <v>1.2755929561765801E-3</v>
+      </c>
       <c r="AF25" s="7" t="s">
         <v>14</v>
       </c>
@@ -3289,10 +3531,18 @@
       <c r="Z26" s="5">
         <v>1.08728955756456E-3</v>
       </c>
-      <c r="AB26" s="2"/>
-      <c r="AC26" s="7"/>
-      <c r="AD26" s="7"/>
-      <c r="AE26" s="7"/>
+      <c r="AB26" t="s">
+        <v>47</v>
+      </c>
+      <c r="AC26">
+        <v>1.3976452487967301E-3</v>
+      </c>
+      <c r="AD26" t="s">
+        <v>45</v>
+      </c>
+      <c r="AE26">
+        <v>1.27243709263701E-3</v>
+      </c>
       <c r="AF26" s="7" t="s">
         <v>50</v>
       </c>
@@ -3391,10 +3641,18 @@
       <c r="Z27" s="5">
         <v>6.9229301091122599E-4</v>
       </c>
-      <c r="AB27" s="2"/>
-      <c r="AC27" s="7"/>
-      <c r="AD27" s="7"/>
-      <c r="AE27" s="7"/>
+      <c r="AB27" t="s">
+        <v>24</v>
+      </c>
+      <c r="AC27">
+        <v>1.39089348522412E-3</v>
+      </c>
+      <c r="AD27" t="s">
+        <v>26</v>
+      </c>
+      <c r="AE27">
+        <v>1.26650553093781E-3</v>
+      </c>
       <c r="AF27" s="7" t="s">
         <v>61</v>
       </c>
@@ -3493,10 +3751,18 @@
       <c r="Z28" s="5">
         <v>5.2506431454673002E-4</v>
       </c>
-      <c r="AB28" s="2"/>
-      <c r="AC28" s="7"/>
-      <c r="AD28" s="7"/>
-      <c r="AE28" s="7"/>
+      <c r="AB28" t="s">
+        <v>14</v>
+      </c>
+      <c r="AC28">
+        <v>1.3563257263990299E-3</v>
+      </c>
+      <c r="AD28" t="s">
+        <v>22</v>
+      </c>
+      <c r="AE28">
+        <v>1.18988818033414E-3</v>
+      </c>
       <c r="AF28" s="7" t="s">
         <v>24</v>
       </c>
@@ -3595,10 +3861,18 @@
       <c r="Z29" s="5">
         <v>3.43953873987734E-4</v>
       </c>
-      <c r="AB29" s="2"/>
-      <c r="AC29" s="7"/>
-      <c r="AD29" s="7"/>
-      <c r="AE29" s="7"/>
+      <c r="AB29" t="s">
+        <v>31</v>
+      </c>
+      <c r="AC29">
+        <v>1.30932832873223E-3</v>
+      </c>
+      <c r="AD29" t="s">
+        <v>20</v>
+      </c>
+      <c r="AE29">
+        <v>1.18881500077817E-3</v>
+      </c>
       <c r="AF29" s="7" t="s">
         <v>23</v>
       </c>
@@ -3697,11 +3971,19 @@
       <c r="Z30" s="5">
         <v>3.1930415373517798E-4</v>
       </c>
-      <c r="AB30" s="2"/>
-      <c r="AC30" s="7"/>
-      <c r="AD30" s="7"/>
-      <c r="AE30" s="7"/>
-      <c r="AF30" s="7" t="s">
+      <c r="AB30" t="s">
+        <v>46</v>
+      </c>
+      <c r="AC30">
+        <v>1.27641236123749E-3</v>
+      </c>
+      <c r="AD30" t="s">
+        <v>14</v>
+      </c>
+      <c r="AE30">
+        <v>1.1674157214620899E-3</v>
+      </c>
+      <c r="AF30" s="32" t="s">
         <v>13</v>
       </c>
       <c r="AG30" s="7">
@@ -3799,10 +4081,18 @@
       <c r="Z31" s="5">
         <v>3.1455495017329501E-4</v>
       </c>
-      <c r="AB31" s="2"/>
-      <c r="AC31" s="7"/>
-      <c r="AD31" s="7"/>
-      <c r="AE31" s="7"/>
+      <c r="AB31" t="s">
+        <v>36</v>
+      </c>
+      <c r="AC31">
+        <v>1.2524106593180999E-3</v>
+      </c>
+      <c r="AD31" t="s">
+        <v>37</v>
+      </c>
+      <c r="AE31">
+        <v>1.1459546090187001E-3</v>
+      </c>
       <c r="AF31" s="7" t="s">
         <v>35</v>
       </c>
@@ -3859,7 +4149,7 @@
       <c r="K32" s="7">
         <v>1.42157466147129E-2</v>
       </c>
-      <c r="L32" s="7" t="s">
+      <c r="L32" s="29" t="s">
         <v>12</v>
       </c>
       <c r="M32" s="5">
@@ -3901,10 +4191,18 @@
       <c r="Z32" s="5">
         <v>1.5968773632843899E-4</v>
       </c>
-      <c r="AB32" s="2"/>
-      <c r="AC32" s="7"/>
-      <c r="AD32" s="7"/>
-      <c r="AE32" s="7"/>
+      <c r="AB32" t="s">
+        <v>30</v>
+      </c>
+      <c r="AC32">
+        <v>1.20219917600766E-3</v>
+      </c>
+      <c r="AD32" t="s">
+        <v>40</v>
+      </c>
+      <c r="AE32">
+        <v>1.1380992175698899E-3</v>
+      </c>
       <c r="AF32" s="7" t="s">
         <v>51</v>
       </c>
@@ -4003,10 +4301,18 @@
       <c r="Z33" s="11">
         <v>6.7196507636513295E-5</v>
       </c>
-      <c r="AB33" s="2"/>
-      <c r="AC33" s="7"/>
-      <c r="AD33" s="7"/>
-      <c r="AE33" s="7"/>
+      <c r="AB33" t="s">
+        <v>15</v>
+      </c>
+      <c r="AC33">
+        <v>1.1654543269679701E-3</v>
+      </c>
+      <c r="AD33" t="s">
+        <v>17</v>
+      </c>
+      <c r="AE33">
+        <v>1.0191962294252301E-3</v>
+      </c>
       <c r="AF33" s="7" t="s">
         <v>66</v>
       </c>
@@ -4105,10 +4411,18 @@
       <c r="Z34" s="11">
         <v>4.2484167039047398E-5</v>
       </c>
-      <c r="AB34" s="2"/>
-      <c r="AC34" s="7"/>
-      <c r="AD34" s="7"/>
-      <c r="AE34" s="7"/>
+      <c r="AB34" t="s">
+        <v>43</v>
+      </c>
+      <c r="AC34">
+        <v>1.1089730444360001E-3</v>
+      </c>
+      <c r="AD34" t="s">
+        <v>15</v>
+      </c>
+      <c r="AE34">
+        <v>1.0014724487669301E-3</v>
+      </c>
       <c r="AF34" s="7" t="s">
         <v>43</v>
       </c>
@@ -4207,10 +4521,18 @@
       <c r="Z35" s="11">
         <v>3.1633549726128801E-5</v>
       </c>
-      <c r="AB35" s="2"/>
-      <c r="AC35" s="7"/>
-      <c r="AD35" s="7"/>
-      <c r="AE35" s="7"/>
+      <c r="AB35" t="s">
+        <v>42</v>
+      </c>
+      <c r="AC35">
+        <v>1.1049985270500801E-3</v>
+      </c>
+      <c r="AD35" t="s">
+        <v>36</v>
+      </c>
+      <c r="AE35">
+        <v>9.4235487819919301E-4</v>
+      </c>
       <c r="AF35" s="7" t="s">
         <v>37</v>
       </c>
@@ -4229,7 +4551,7 @@
       <c r="AK35" s="7">
         <v>2.7465018431786599E-3</v>
       </c>
-      <c r="AL35" s="7" t="s">
+      <c r="AL35" s="40" t="s">
         <v>32</v>
       </c>
       <c r="AM35" s="5">
@@ -4309,10 +4631,18 @@
       <c r="Z36" s="11">
         <v>1.6782943256643501E-5</v>
       </c>
-      <c r="AB36" s="2"/>
-      <c r="AC36" s="7"/>
-      <c r="AD36" s="7"/>
-      <c r="AE36" s="7"/>
+      <c r="AB36" t="s">
+        <v>25</v>
+      </c>
+      <c r="AC36">
+        <v>1.0048767832882301E-3</v>
+      </c>
+      <c r="AD36" t="s">
+        <v>39</v>
+      </c>
+      <c r="AE36">
+        <v>9.3303192552681498E-4</v>
+      </c>
       <c r="AF36" s="7" t="s">
         <v>15</v>
       </c>
@@ -4411,10 +4741,18 @@
       <c r="Z37" s="11">
         <v>1.39843735386779E-5</v>
       </c>
-      <c r="AB37" s="2"/>
-      <c r="AC37" s="7"/>
-      <c r="AD37" s="7"/>
-      <c r="AE37" s="7"/>
+      <c r="AB37" t="s">
+        <v>50</v>
+      </c>
+      <c r="AC37">
+        <v>9.9929841976359999E-4</v>
+      </c>
+      <c r="AD37" t="s">
+        <v>51</v>
+      </c>
+      <c r="AE37">
+        <v>8.9920974779855397E-4</v>
+      </c>
       <c r="AF37" s="7" t="s">
         <v>53</v>
       </c>
@@ -4513,10 +4851,18 @@
       <c r="Z38" s="11">
         <v>8.6838322268523104E-6</v>
       </c>
-      <c r="AB38" s="2"/>
-      <c r="AC38" s="7"/>
-      <c r="AD38" s="7"/>
-      <c r="AE38" s="7"/>
+      <c r="AB38" t="s">
+        <v>48</v>
+      </c>
+      <c r="AC38">
+        <v>9.40009241809762E-4</v>
+      </c>
+      <c r="AD38" t="s">
+        <v>46</v>
+      </c>
+      <c r="AE38">
+        <v>8.9739354833706295E-4</v>
+      </c>
       <c r="AF38" s="7" t="s">
         <v>29</v>
       </c>
@@ -4615,10 +4961,18 @@
       <c r="Z39" s="5">
         <v>0</v>
       </c>
-      <c r="AB39" s="2"/>
-      <c r="AC39" s="7"/>
-      <c r="AD39" s="7"/>
-      <c r="AE39" s="7"/>
+      <c r="AB39" t="s">
+        <v>40</v>
+      </c>
+      <c r="AC39">
+        <v>9.1961378181067404E-4</v>
+      </c>
+      <c r="AD39" t="s">
+        <v>25</v>
+      </c>
+      <c r="AE39">
+        <v>8.9723999747982799E-4</v>
+      </c>
       <c r="AF39" s="7" t="s">
         <v>60</v>
       </c>
@@ -4637,7 +4991,7 @@
       <c r="AK39" s="7">
         <v>2.11694217445999E-3</v>
       </c>
-      <c r="AL39" s="7" t="s">
+      <c r="AL39" s="40" t="s">
         <v>46</v>
       </c>
       <c r="AM39" s="5">
@@ -4717,10 +5071,18 @@
       <c r="Z40" s="5">
         <v>0</v>
       </c>
-      <c r="AB40" s="2"/>
-      <c r="AC40" s="7"/>
-      <c r="AD40" s="7"/>
-      <c r="AE40" s="7"/>
+      <c r="AB40" t="s">
+        <v>19</v>
+      </c>
+      <c r="AC40">
+        <v>9.1261239512190203E-4</v>
+      </c>
+      <c r="AD40" t="s">
+        <v>35</v>
+      </c>
+      <c r="AE40">
+        <v>8.6298487428190503E-4</v>
+      </c>
       <c r="AF40" s="7" t="s">
         <v>46</v>
       </c>
@@ -4819,10 +5181,18 @@
       <c r="Z41" s="5">
         <v>0</v>
       </c>
-      <c r="AB41" s="2"/>
-      <c r="AC41" s="7"/>
-      <c r="AD41" s="7"/>
-      <c r="AE41" s="7"/>
+      <c r="AB41" t="s">
+        <v>17</v>
+      </c>
+      <c r="AC41">
+        <v>9.1148823419837403E-4</v>
+      </c>
+      <c r="AD41" t="s">
+        <v>44</v>
+      </c>
+      <c r="AE41">
+        <v>8.3701149240452799E-4</v>
+      </c>
       <c r="AF41" s="7" t="s">
         <v>48</v>
       </c>
@@ -4921,10 +5291,18 @@
       <c r="Z42" s="5">
         <v>0</v>
       </c>
-      <c r="AB42" s="2"/>
-      <c r="AC42" s="7"/>
-      <c r="AD42" s="7"/>
-      <c r="AE42" s="7"/>
+      <c r="AB42" t="s">
+        <v>49</v>
+      </c>
+      <c r="AC42">
+        <v>8.6769451481948502E-4</v>
+      </c>
+      <c r="AD42" t="s">
+        <v>49</v>
+      </c>
+      <c r="AE42">
+        <v>7.88224211093635E-4</v>
+      </c>
       <c r="AF42" s="7" t="s">
         <v>57</v>
       </c>
@@ -5023,10 +5401,18 @@
       <c r="Z43" s="5">
         <v>0</v>
       </c>
-      <c r="AB43" s="2"/>
-      <c r="AC43" s="7"/>
-      <c r="AD43" s="7"/>
-      <c r="AE43" s="7"/>
+      <c r="AB43" t="s">
+        <v>63</v>
+      </c>
+      <c r="AC43">
+        <v>8.6438186435904897E-4</v>
+      </c>
+      <c r="AD43" t="s">
+        <v>53</v>
+      </c>
+      <c r="AE43">
+        <v>7.8287179963565205E-4</v>
+      </c>
       <c r="AF43" s="7" t="s">
         <v>19</v>
       </c>
@@ -5125,10 +5511,18 @@
       <c r="Z44" s="5">
         <v>0</v>
       </c>
-      <c r="AB44" s="2"/>
-      <c r="AC44" s="7"/>
-      <c r="AD44" s="7"/>
-      <c r="AE44" s="7"/>
+      <c r="AB44" t="s">
+        <v>44</v>
+      </c>
+      <c r="AC44">
+        <v>8.3208925594835902E-4</v>
+      </c>
+      <c r="AD44" t="s">
+        <v>47</v>
+      </c>
+      <c r="AE44">
+        <v>7.7800350180467701E-4</v>
+      </c>
       <c r="AF44" s="7" t="s">
         <v>70</v>
       </c>
@@ -5227,10 +5621,18 @@
       <c r="Z45" s="5">
         <v>0</v>
       </c>
-      <c r="AB45" s="2"/>
-      <c r="AC45" s="7"/>
-      <c r="AD45" s="7"/>
-      <c r="AE45" s="7"/>
+      <c r="AB45" t="s">
+        <v>53</v>
+      </c>
+      <c r="AC45">
+        <v>8.2952394190677402E-4</v>
+      </c>
+      <c r="AD45" t="s">
+        <v>58</v>
+      </c>
+      <c r="AE45">
+        <v>6.7215561217786202E-4</v>
+      </c>
       <c r="AF45" s="7" t="s">
         <v>49</v>
       </c>
@@ -5329,10 +5731,18 @@
       <c r="Z46" s="5">
         <v>0</v>
       </c>
-      <c r="AB46" s="2"/>
-      <c r="AC46" s="7"/>
-      <c r="AD46" s="7"/>
-      <c r="AE46" s="7"/>
+      <c r="AB46" t="s">
+        <v>61</v>
+      </c>
+      <c r="AC46">
+        <v>7.6953426094541197E-4</v>
+      </c>
+      <c r="AD46" t="s">
+        <v>55</v>
+      </c>
+      <c r="AE46">
+        <v>6.6929312042476896E-4</v>
+      </c>
       <c r="AF46" s="7" t="s">
         <v>31</v>
       </c>
@@ -5431,10 +5841,18 @@
       <c r="Z47" s="5">
         <v>0</v>
       </c>
-      <c r="AB47" s="2"/>
-      <c r="AC47" s="7"/>
-      <c r="AD47" s="7"/>
-      <c r="AE47" s="7"/>
+      <c r="AB47" t="s">
+        <v>57</v>
+      </c>
+      <c r="AC47">
+        <v>7.2209619170290201E-4</v>
+      </c>
+      <c r="AD47" t="s">
+        <v>57</v>
+      </c>
+      <c r="AE47">
+        <v>6.5004131873519901E-4</v>
+      </c>
       <c r="AF47" s="7" t="s">
         <v>36</v>
       </c>
@@ -5533,10 +5951,18 @@
       <c r="Z48" s="11">
         <v>-1.4461255599673701E-5</v>
       </c>
-      <c r="AB48" s="2"/>
-      <c r="AC48" s="7"/>
-      <c r="AD48" s="7"/>
-      <c r="AE48" s="7"/>
+      <c r="AB48" t="s">
+        <v>60</v>
+      </c>
+      <c r="AC48">
+        <v>7.1573651154714798E-4</v>
+      </c>
+      <c r="AD48" t="s">
+        <v>54</v>
+      </c>
+      <c r="AE48">
+        <v>6.4456228821977704E-4</v>
+      </c>
       <c r="AF48" s="7" t="s">
         <v>17</v>
       </c>
@@ -5635,10 +6061,18 @@
       <c r="Z49" s="11">
         <v>-4.2148014296827797E-5</v>
       </c>
-      <c r="AB49" s="2"/>
-      <c r="AC49" s="7"/>
-      <c r="AD49" s="7"/>
-      <c r="AE49" s="7"/>
+      <c r="AB49" t="s">
+        <v>55</v>
+      </c>
+      <c r="AC49">
+        <v>7.1291005594875602E-4</v>
+      </c>
+      <c r="AD49" t="s">
+        <v>41</v>
+      </c>
+      <c r="AE49">
+        <v>5.8264473111652398E-4</v>
+      </c>
       <c r="AF49" s="7" t="s">
         <v>41</v>
       </c>
@@ -5737,10 +6171,18 @@
       <c r="Z50" s="11">
         <v>-5.1759028130726701E-5</v>
       </c>
-      <c r="AB50" s="2"/>
-      <c r="AC50" s="7"/>
-      <c r="AD50" s="7"/>
-      <c r="AE50" s="7"/>
+      <c r="AB50" t="s">
+        <v>52</v>
+      </c>
+      <c r="AC50">
+        <v>7.1246105470053605E-4</v>
+      </c>
+      <c r="AD50" t="s">
+        <v>63</v>
+      </c>
+      <c r="AE50">
+        <v>5.7322466738534902E-4</v>
+      </c>
       <c r="AF50" s="7" t="s">
         <v>58</v>
       </c>
@@ -5839,10 +6281,18 @@
       <c r="Z51" s="11">
         <v>-9.0887216161661405E-5</v>
       </c>
-      <c r="AB51" s="2"/>
-      <c r="AC51" s="7"/>
-      <c r="AD51" s="7"/>
-      <c r="AE51" s="7"/>
+      <c r="AB51" t="s">
+        <v>35</v>
+      </c>
+      <c r="AC51">
+        <v>7.0073361910033896E-4</v>
+      </c>
+      <c r="AD51" t="s">
+        <v>52</v>
+      </c>
+      <c r="AE51">
+        <v>5.2189888662750896E-4</v>
+      </c>
       <c r="AF51" s="7" t="s">
         <v>47</v>
       </c>
@@ -5941,10 +6391,18 @@
       <c r="Z52" s="5">
         <v>-3.4441034849397301E-4</v>
       </c>
-      <c r="AB52" s="2"/>
-      <c r="AC52" s="7"/>
-      <c r="AD52" s="7"/>
-      <c r="AE52" s="7"/>
+      <c r="AB52" t="s">
+        <v>51</v>
+      </c>
+      <c r="AC52">
+        <v>6.9084907638659605E-4</v>
+      </c>
+      <c r="AD52" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE52">
+        <v>5.12651551744207E-4</v>
+      </c>
       <c r="AF52" s="7" t="s">
         <v>68</v>
       </c>
@@ -6043,10 +6501,18 @@
       <c r="Z53" s="5">
         <v>-4.2362561524282799E-4</v>
       </c>
-      <c r="AB53" s="2"/>
-      <c r="AC53" s="7"/>
-      <c r="AD53" s="7"/>
-      <c r="AE53" s="7"/>
+      <c r="AB53" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC53">
+        <v>6.3960143103651004E-4</v>
+      </c>
+      <c r="AD53" t="s">
+        <v>48</v>
+      </c>
+      <c r="AE53">
+        <v>5.0063266569698895E-4</v>
+      </c>
       <c r="AF53" s="7" t="s">
         <v>21</v>
       </c>
@@ -6145,10 +6611,18 @@
       <c r="Z54" s="5">
         <v>-5.4323646554812403E-4</v>
       </c>
-      <c r="AB54" s="2"/>
-      <c r="AC54" s="7"/>
-      <c r="AD54" s="7"/>
-      <c r="AE54" s="7"/>
+      <c r="AB54" t="s">
+        <v>56</v>
+      </c>
+      <c r="AC54">
+        <v>5.6408035456857904E-4</v>
+      </c>
+      <c r="AD54" t="s">
+        <v>62</v>
+      </c>
+      <c r="AE54">
+        <v>4.8010032184244599E-4</v>
+      </c>
       <c r="AF54" s="7" t="s">
         <v>73</v>
       </c>
@@ -6247,10 +6721,18 @@
       <c r="Z55" s="5">
         <v>-6.63719710535026E-4</v>
       </c>
-      <c r="AB55" s="2"/>
-      <c r="AC55" s="7"/>
-      <c r="AD55" s="7"/>
-      <c r="AE55" s="7"/>
+      <c r="AB55" t="s">
+        <v>65</v>
+      </c>
+      <c r="AC55">
+        <v>5.4587304723366901E-4</v>
+      </c>
+      <c r="AD55" t="s">
+        <v>56</v>
+      </c>
+      <c r="AE55">
+        <v>4.56921881115847E-4</v>
+      </c>
       <c r="AF55" s="7" t="s">
         <v>59</v>
       </c>
@@ -6349,10 +6831,18 @@
       <c r="Z56" s="5">
         <v>-7.3420959737342502E-4</v>
       </c>
-      <c r="AB56" s="2"/>
-      <c r="AC56" s="7"/>
-      <c r="AD56" s="7"/>
-      <c r="AE56" s="7"/>
+      <c r="AB56" t="s">
+        <v>62</v>
+      </c>
+      <c r="AC56">
+        <v>5.3454927898970096E-4</v>
+      </c>
+      <c r="AD56" t="s">
+        <v>61</v>
+      </c>
+      <c r="AE56">
+        <v>3.8935498678275502E-4</v>
+      </c>
       <c r="AF56" s="7" t="s">
         <v>74</v>
       </c>
@@ -6451,10 +6941,18 @@
       <c r="Z57" s="5">
         <v>-1.00893111508932E-3</v>
       </c>
-      <c r="AB57" s="2"/>
-      <c r="AC57" s="7"/>
-      <c r="AD57" s="7"/>
-      <c r="AE57" s="7"/>
+      <c r="AB57" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC57">
+        <v>5.2749673280973002E-4</v>
+      </c>
+      <c r="AD57" t="s">
+        <v>59</v>
+      </c>
+      <c r="AE57">
+        <v>3.3776296140798103E-4</v>
+      </c>
       <c r="AF57" s="7" t="s">
         <v>33</v>
       </c>
@@ -6553,10 +7051,18 @@
       <c r="Z58" s="5">
         <v>-1.1313624165418801E-3</v>
       </c>
-      <c r="AB58" s="2"/>
-      <c r="AC58" s="7"/>
-      <c r="AD58" s="7"/>
-      <c r="AE58" s="7"/>
+      <c r="AB58" t="s">
+        <v>41</v>
+      </c>
+      <c r="AC58">
+        <v>4.49919511107217E-4</v>
+      </c>
+      <c r="AD58" t="s">
+        <v>65</v>
+      </c>
+      <c r="AE58">
+        <v>3.1367028026863002E-4</v>
+      </c>
       <c r="AF58" s="7" t="s">
         <v>40</v>
       </c>
@@ -6655,10 +7161,18 @@
       <c r="Z59" s="5">
         <v>-1.1651292131859201E-3</v>
       </c>
-      <c r="AB59" s="2"/>
-      <c r="AC59" s="7"/>
-      <c r="AD59" s="7"/>
-      <c r="AE59" s="7"/>
+      <c r="AB59" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC59">
+        <v>3.6806787873451199E-4</v>
+      </c>
+      <c r="AD59" t="s">
+        <v>70</v>
+      </c>
+      <c r="AE59">
+        <v>2.36296916188303E-4</v>
+      </c>
       <c r="AF59" s="7" t="s">
         <v>56</v>
       </c>
@@ -6757,10 +7271,18 @@
       <c r="Z60" s="5">
         <v>-1.2568869391176699E-3</v>
       </c>
-      <c r="AB60" s="2"/>
-      <c r="AC60" s="7"/>
-      <c r="AD60" s="7"/>
-      <c r="AE60" s="7"/>
+      <c r="AB60" t="s">
+        <v>64</v>
+      </c>
+      <c r="AC60">
+        <v>3.1223778752851098E-4</v>
+      </c>
+      <c r="AD60" t="s">
+        <v>77</v>
+      </c>
+      <c r="AE60">
+        <v>2.2683221319616501E-4</v>
+      </c>
       <c r="AF60" s="7" t="s">
         <v>69</v>
       </c>
@@ -6859,10 +7381,18 @@
       <c r="Z61" s="5">
         <v>-1.26832133898302E-3</v>
       </c>
-      <c r="AB61" s="2"/>
-      <c r="AC61" s="7"/>
-      <c r="AD61" s="7"/>
-      <c r="AE61" s="7"/>
+      <c r="AB61" t="s">
+        <v>66</v>
+      </c>
+      <c r="AC61">
+        <v>2.1852006958099899E-4</v>
+      </c>
+      <c r="AD61" t="s">
+        <v>64</v>
+      </c>
+      <c r="AE61">
+        <v>1.8196414585959299E-4</v>
+      </c>
       <c r="AF61" s="7" t="s">
         <v>42</v>
       </c>
@@ -6961,10 +7491,18 @@
       <c r="Z62" s="5">
         <v>-1.3407887486275899E-3</v>
       </c>
-      <c r="AB62" s="2"/>
-      <c r="AC62" s="7"/>
-      <c r="AD62" s="7"/>
-      <c r="AE62" s="7"/>
+      <c r="AB62" t="s">
+        <v>71</v>
+      </c>
+      <c r="AC62">
+        <v>2.0378428364608301E-4</v>
+      </c>
+      <c r="AD62" t="s">
+        <v>71</v>
+      </c>
+      <c r="AE62">
+        <v>1.56236310106821E-4</v>
+      </c>
       <c r="AF62" s="7" t="s">
         <v>71</v>
       </c>
@@ -7063,10 +7601,18 @@
       <c r="Z63" s="5">
         <v>-1.4113426843644901E-3</v>
       </c>
-      <c r="AB63" s="2"/>
-      <c r="AC63" s="7"/>
-      <c r="AD63" s="7"/>
-      <c r="AE63" s="7"/>
+      <c r="AB63" t="s">
+        <v>70</v>
+      </c>
+      <c r="AC63">
+        <v>1.48834690786912E-4</v>
+      </c>
+      <c r="AD63" t="s">
+        <v>66</v>
+      </c>
+      <c r="AE63">
+        <v>1.00189867576008E-4</v>
+      </c>
       <c r="AF63" s="7" t="s">
         <v>26</v>
       </c>
@@ -7165,10 +7711,18 @@
       <c r="Z64" s="5">
         <v>-1.52182389632558E-3</v>
       </c>
-      <c r="AB64" s="2"/>
-      <c r="AC64" s="7"/>
-      <c r="AD64" s="7"/>
-      <c r="AE64" s="7"/>
+      <c r="AB64" t="s">
+        <v>68</v>
+      </c>
+      <c r="AC64">
+        <v>1.2398531710193801E-4</v>
+      </c>
+      <c r="AD64" t="s">
+        <v>67</v>
+      </c>
+      <c r="AE64" s="9">
+        <v>9.9997420337643298E-5</v>
+      </c>
       <c r="AF64" s="7" t="s">
         <v>55</v>
       </c>
@@ -7267,10 +7821,18 @@
       <c r="Z65" s="5">
         <v>-1.6854042546383199E-3</v>
       </c>
-      <c r="AB65" s="2"/>
-      <c r="AC65" s="7"/>
-      <c r="AD65" s="7"/>
-      <c r="AE65" s="7"/>
+      <c r="AB65" t="s">
+        <v>72</v>
+      </c>
+      <c r="AC65">
+        <v>1.04688748483742E-4</v>
+      </c>
+      <c r="AD65" t="s">
+        <v>68</v>
+      </c>
+      <c r="AE65" s="9">
+        <v>7.2275757972106597E-5</v>
+      </c>
       <c r="AF65" s="7" t="s">
         <v>83</v>
       </c>
@@ -7369,10 +7931,18 @@
       <c r="Z66" s="5">
         <v>-2.0310813820381499E-3</v>
       </c>
-      <c r="AB66" s="2"/>
-      <c r="AC66" s="7"/>
-      <c r="AD66" s="7"/>
-      <c r="AE66" s="7"/>
+      <c r="AB66" t="s">
+        <v>73</v>
+      </c>
+      <c r="AC66" s="9">
+        <v>9.5338462083283001E-5</v>
+      </c>
+      <c r="AD66" t="s">
+        <v>73</v>
+      </c>
+      <c r="AE66" s="9">
+        <v>6.8897718624410495E-5</v>
+      </c>
       <c r="AF66" s="7" t="s">
         <v>72</v>
       </c>
@@ -7471,10 +8041,18 @@
       <c r="Z67" s="5">
         <v>-2.3136124014424102E-3</v>
       </c>
-      <c r="AB67" s="2"/>
-      <c r="AC67" s="7"/>
-      <c r="AD67" s="7"/>
-      <c r="AE67" s="7"/>
+      <c r="AB67" t="s">
+        <v>69</v>
+      </c>
+      <c r="AC67" s="9">
+        <v>7.7628583109150398E-5</v>
+      </c>
+      <c r="AD67" t="s">
+        <v>72</v>
+      </c>
+      <c r="AE67" s="9">
+        <v>6.2613684707430204E-5</v>
+      </c>
       <c r="AF67" s="7" t="s">
         <v>54</v>
       </c>
@@ -7573,10 +8151,18 @@
       <c r="Z68" s="5">
         <v>-2.4402964824282E-3</v>
       </c>
-      <c r="AB68" s="2"/>
-      <c r="AC68" s="7"/>
-      <c r="AD68" s="7"/>
-      <c r="AE68" s="7"/>
+      <c r="AB68" t="s">
+        <v>67</v>
+      </c>
+      <c r="AC68" s="9">
+        <v>7.5813302271829095E-5</v>
+      </c>
+      <c r="AD68" t="s">
+        <v>82</v>
+      </c>
+      <c r="AE68" s="9">
+        <v>5.0964012611896799E-5</v>
+      </c>
       <c r="AF68" s="7" t="s">
         <v>85</v>
       </c>
@@ -7675,10 +8261,18 @@
       <c r="Z69" s="5">
         <v>-3.2517459752786399E-3</v>
       </c>
-      <c r="AB69" s="2"/>
-      <c r="AC69" s="7"/>
-      <c r="AD69" s="7"/>
-      <c r="AE69" s="7"/>
+      <c r="AB69" t="s">
+        <v>74</v>
+      </c>
+      <c r="AC69" s="9">
+        <v>5.7624940449316501E-5</v>
+      </c>
+      <c r="AD69" t="s">
+        <v>79</v>
+      </c>
+      <c r="AE69" s="9">
+        <v>4.2918755706986902E-5</v>
+      </c>
       <c r="AF69" s="7" t="s">
         <v>81</v>
       </c>
@@ -7777,10 +8371,18 @@
       <c r="Z70" s="5">
         <v>-3.7711695951458501E-3</v>
       </c>
-      <c r="AB70" s="2"/>
-      <c r="AC70" s="7"/>
-      <c r="AD70" s="7"/>
-      <c r="AE70" s="7"/>
+      <c r="AB70" t="s">
+        <v>77</v>
+      </c>
+      <c r="AC70" s="9">
+        <v>5.2403151939373002E-5</v>
+      </c>
+      <c r="AD70" t="s">
+        <v>80</v>
+      </c>
+      <c r="AE70" s="9">
+        <v>3.02957667463319E-5</v>
+      </c>
       <c r="AF70" s="7" t="s">
         <v>44</v>
       </c>
@@ -7879,10 +8481,18 @@
       <c r="Z71" s="5">
         <v>-4.0167708042509699E-3</v>
       </c>
-      <c r="AB71" s="2"/>
-      <c r="AC71" s="7"/>
-      <c r="AD71" s="7"/>
-      <c r="AE71" s="7"/>
+      <c r="AB71" t="s">
+        <v>75</v>
+      </c>
+      <c r="AC71" s="9">
+        <v>2.6728088356225899E-5</v>
+      </c>
+      <c r="AD71" t="s">
+        <v>76</v>
+      </c>
+      <c r="AE71" s="9">
+        <v>2.99235011597841E-5</v>
+      </c>
       <c r="AF71" s="7" t="s">
         <v>84</v>
       </c>
@@ -7981,10 +8591,18 @@
       <c r="Z72" s="5">
         <v>-5.0805827180908604E-3</v>
       </c>
-      <c r="AB72" s="2"/>
-      <c r="AC72" s="7"/>
-      <c r="AD72" s="7"/>
-      <c r="AE72" s="7"/>
+      <c r="AB72" t="s">
+        <v>80</v>
+      </c>
+      <c r="AC72" s="9">
+        <v>2.6643386490152899E-5</v>
+      </c>
+      <c r="AD72" t="s">
+        <v>69</v>
+      </c>
+      <c r="AE72" s="9">
+        <v>2.29599147030014E-5</v>
+      </c>
       <c r="AF72" s="7" t="s">
         <v>79</v>
       </c>
@@ -8083,10 +8701,18 @@
       <c r="Z73" s="5">
         <v>-5.77651972972774E-3</v>
       </c>
-      <c r="AB73" s="2"/>
-      <c r="AC73" s="7"/>
-      <c r="AD73" s="7"/>
-      <c r="AE73" s="7"/>
+      <c r="AB73" t="s">
+        <v>79</v>
+      </c>
+      <c r="AC73" s="9">
+        <v>2.6290742326931299E-5</v>
+      </c>
+      <c r="AD73" t="s">
+        <v>83</v>
+      </c>
+      <c r="AE73" s="9">
+        <v>1.00689309300377E-5</v>
+      </c>
       <c r="AF73" s="7" t="s">
         <v>82</v>
       </c>
@@ -8185,10 +8811,18 @@
       <c r="Z74" s="5">
         <v>-6.1812156547884998E-3</v>
       </c>
-      <c r="AB74" s="2"/>
-      <c r="AC74" s="7"/>
-      <c r="AD74" s="7"/>
-      <c r="AE74" s="7"/>
+      <c r="AB74" t="s">
+        <v>76</v>
+      </c>
+      <c r="AC74" s="9">
+        <v>2.4963505678397699E-5</v>
+      </c>
+      <c r="AD74" t="s">
+        <v>75</v>
+      </c>
+      <c r="AE74" s="9">
+        <v>9.3710521130025599E-6</v>
+      </c>
       <c r="AF74" s="7" t="s">
         <v>80</v>
       </c>
@@ -8287,10 +8921,18 @@
       <c r="Z75" s="5">
         <v>-8.7323495979083603E-3</v>
       </c>
-      <c r="AB75" s="2"/>
-      <c r="AC75" s="7"/>
-      <c r="AD75" s="7"/>
-      <c r="AE75" s="7"/>
+      <c r="AB75" t="s">
+        <v>81</v>
+      </c>
+      <c r="AC75" s="9">
+        <v>1.57393746125837E-5</v>
+      </c>
+      <c r="AD75" t="s">
+        <v>81</v>
+      </c>
+      <c r="AE75" s="9">
+        <v>8.9050795247180505E-6</v>
+      </c>
       <c r="AF75" s="7" t="s">
         <v>87</v>
       </c>
@@ -8389,10 +9031,18 @@
       <c r="Z76" s="5">
         <v>-1.1072898074557899E-2</v>
       </c>
-      <c r="AB76" s="2"/>
-      <c r="AC76" s="7"/>
-      <c r="AD76" s="7"/>
-      <c r="AE76" s="7"/>
+      <c r="AB76" t="s">
+        <v>82</v>
+      </c>
+      <c r="AC76" s="9">
+        <v>9.4633533883454003E-6</v>
+      </c>
+      <c r="AD76" t="s">
+        <v>74</v>
+      </c>
+      <c r="AE76" s="9">
+        <v>5.7553114082644001E-6</v>
+      </c>
       <c r="AF76" s="7" t="s">
         <v>77</v>
       </c>
@@ -8491,10 +9141,18 @@
       <c r="Z77" s="5">
         <v>-1.20917274753166E-2</v>
       </c>
-      <c r="AB77" s="2"/>
-      <c r="AC77" s="7"/>
-      <c r="AD77" s="7"/>
-      <c r="AE77" s="7"/>
+      <c r="AB77" t="s">
+        <v>83</v>
+      </c>
+      <c r="AC77" s="9">
+        <v>6.6821874744393596E-6</v>
+      </c>
+      <c r="AD77" t="s">
+        <v>84</v>
+      </c>
+      <c r="AE77" s="9">
+        <v>3.2036575940689201E-6</v>
+      </c>
       <c r="AF77" s="7" t="s">
         <v>75</v>
       </c>
@@ -8593,10 +9251,18 @@
       <c r="Z78" s="5">
         <v>-1.5969336102454199E-2</v>
       </c>
-      <c r="AB78" s="2"/>
-      <c r="AC78" s="7"/>
-      <c r="AD78" s="7"/>
-      <c r="AE78" s="7"/>
+      <c r="AB78" t="s">
+        <v>78</v>
+      </c>
+      <c r="AC78" s="9">
+        <v>4.9719229329042699E-6</v>
+      </c>
+      <c r="AD78" t="s">
+        <v>78</v>
+      </c>
+      <c r="AE78" s="9">
+        <v>3.1828419351976098E-6</v>
+      </c>
       <c r="AF78" s="7" t="s">
         <v>67</v>
       </c>
@@ -8695,10 +9361,18 @@
       <c r="Z79" s="5">
         <v>-2.32614359001025E-2</v>
       </c>
-      <c r="AB79" s="2"/>
-      <c r="AC79" s="7"/>
-      <c r="AD79" s="7"/>
-      <c r="AE79" s="7"/>
+      <c r="AB79" t="s">
+        <v>84</v>
+      </c>
+      <c r="AC79" s="9">
+        <v>4.31657319380512E-6</v>
+      </c>
+      <c r="AD79" t="s">
+        <v>87</v>
+      </c>
+      <c r="AE79" s="9">
+        <v>2.0074050123623501E-6</v>
+      </c>
       <c r="AF79" s="7" t="s">
         <v>78</v>
       </c>
@@ -8797,10 +9471,18 @@
       <c r="Z80" s="5">
         <v>-2.9240400740999699E-2</v>
       </c>
-      <c r="AB80" s="2"/>
-      <c r="AC80" s="7"/>
-      <c r="AD80" s="7"/>
-      <c r="AE80" s="7"/>
+      <c r="AB80" t="s">
+        <v>85</v>
+      </c>
+      <c r="AC80" s="9">
+        <v>3.36804974572022E-6</v>
+      </c>
+      <c r="AD80" t="s">
+        <v>85</v>
+      </c>
+      <c r="AE80" s="9">
+        <v>1.07938820904232E-6</v>
+      </c>
       <c r="AF80" s="7" t="s">
         <v>76</v>
       </c>
@@ -8883,10 +9565,18 @@
       <c r="X81" s="7"/>
       <c r="Y81" s="7"/>
       <c r="Z81" s="5"/>
-      <c r="AB81" s="2"/>
-      <c r="AC81" s="7"/>
-      <c r="AD81" s="7"/>
-      <c r="AE81" s="7"/>
+      <c r="AB81" t="s">
+        <v>87</v>
+      </c>
+      <c r="AC81" s="9">
+        <v>3.2103745053004701E-6</v>
+      </c>
+      <c r="AD81" t="s">
+        <v>86</v>
+      </c>
+      <c r="AE81" s="9">
+        <v>5.2694578094360998E-7</v>
+      </c>
       <c r="AF81" s="7" t="s">
         <v>86</v>
       </c>
@@ -8937,21 +9627,15 @@
       <c r="X82" s="7"/>
       <c r="Y82" s="7"/>
       <c r="Z82" s="5"/>
+      <c r="AB82" t="s">
+        <v>86</v>
+      </c>
+      <c r="AC82" s="9">
+        <v>7.1131721892138101E-7</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="AB3:AC3"/>
-    <mergeCell ref="AD3:AE3"/>
-    <mergeCell ref="AF3:AG3"/>
-    <mergeCell ref="AH3:AI3"/>
-    <mergeCell ref="AJ3:AK3"/>
-    <mergeCell ref="AL3:AM3"/>
-    <mergeCell ref="O3:P3"/>
-    <mergeCell ref="Q3:R3"/>
-    <mergeCell ref="S3:T3"/>
-    <mergeCell ref="U3:V3"/>
-    <mergeCell ref="W3:X3"/>
-    <mergeCell ref="Y3:Z3"/>
     <mergeCell ref="B2:M2"/>
     <mergeCell ref="O2:Z2"/>
     <mergeCell ref="AB2:AM2"/>
@@ -8961,6 +9645,18 @@
     <mergeCell ref="H3:I3"/>
     <mergeCell ref="J3:K3"/>
     <mergeCell ref="L3:M3"/>
+    <mergeCell ref="AL3:AM3"/>
+    <mergeCell ref="O3:P3"/>
+    <mergeCell ref="Q3:R3"/>
+    <mergeCell ref="S3:T3"/>
+    <mergeCell ref="U3:V3"/>
+    <mergeCell ref="W3:X3"/>
+    <mergeCell ref="Y3:Z3"/>
+    <mergeCell ref="AB3:AC3"/>
+    <mergeCell ref="AD3:AE3"/>
+    <mergeCell ref="AF3:AG3"/>
+    <mergeCell ref="AH3:AI3"/>
+    <mergeCell ref="AJ3:AK3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -8990,147 +9686,147 @@
   <sheetData>
     <row r="1" spans="2:43" ht="5" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="2" spans="2:43" x14ac:dyDescent="0.2">
-      <c r="B2" s="17" t="s">
+      <c r="B2" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="18"/>
-      <c r="D2" s="18"/>
-      <c r="E2" s="18"/>
-      <c r="F2" s="18"/>
-      <c r="G2" s="19"/>
+      <c r="C2" s="21"/>
+      <c r="D2" s="21"/>
+      <c r="E2" s="21"/>
+      <c r="F2" s="21"/>
+      <c r="G2" s="22"/>
       <c r="H2" s="3"/>
-      <c r="I2" s="17" t="s">
+      <c r="I2" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="J2" s="18"/>
-      <c r="K2" s="18"/>
-      <c r="L2" s="18"/>
-      <c r="M2" s="18"/>
-      <c r="N2" s="19"/>
+      <c r="J2" s="21"/>
+      <c r="K2" s="21"/>
+      <c r="L2" s="21"/>
+      <c r="M2" s="21"/>
+      <c r="N2" s="22"/>
       <c r="O2" s="3"/>
-      <c r="P2" s="17" t="s">
+      <c r="P2" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="Q2" s="18"/>
-      <c r="R2" s="18"/>
-      <c r="S2" s="18"/>
-      <c r="T2" s="18"/>
-      <c r="U2" s="19"/>
+      <c r="Q2" s="21"/>
+      <c r="R2" s="21"/>
+      <c r="S2" s="21"/>
+      <c r="T2" s="21"/>
+      <c r="U2" s="22"/>
       <c r="V2" s="3"/>
-      <c r="W2" s="17" t="s">
+      <c r="W2" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="X2" s="18"/>
-      <c r="Y2" s="18"/>
-      <c r="Z2" s="18"/>
-      <c r="AA2" s="18"/>
-      <c r="AB2" s="19"/>
+      <c r="X2" s="21"/>
+      <c r="Y2" s="21"/>
+      <c r="Z2" s="21"/>
+      <c r="AA2" s="21"/>
+      <c r="AB2" s="22"/>
       <c r="AC2" s="3"/>
-      <c r="AD2" s="17" t="s">
+      <c r="AD2" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="AE2" s="18"/>
-      <c r="AF2" s="18"/>
-      <c r="AG2" s="18"/>
-      <c r="AH2" s="18"/>
-      <c r="AI2" s="19"/>
+      <c r="AE2" s="21"/>
+      <c r="AF2" s="21"/>
+      <c r="AG2" s="21"/>
+      <c r="AH2" s="21"/>
+      <c r="AI2" s="22"/>
       <c r="AJ2" s="3"/>
-      <c r="AK2" s="17" t="s">
+      <c r="AK2" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="AL2" s="18"/>
-      <c r="AM2" s="18"/>
-      <c r="AN2" s="18"/>
-      <c r="AO2" s="18"/>
-      <c r="AP2" s="19"/>
+      <c r="AL2" s="21"/>
+      <c r="AM2" s="21"/>
+      <c r="AN2" s="21"/>
+      <c r="AO2" s="21"/>
+      <c r="AP2" s="22"/>
       <c r="AQ2" s="8"/>
     </row>
     <row r="3" spans="2:43" x14ac:dyDescent="0.2">
-      <c r="B3" s="12" t="s">
+      <c r="B3" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="13"/>
-      <c r="D3" s="13" t="s">
+      <c r="C3" s="17"/>
+      <c r="D3" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="13"/>
-      <c r="F3" s="13" t="s">
+      <c r="E3" s="17"/>
+      <c r="F3" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="G3" s="14"/>
-      <c r="I3" s="12" t="s">
+      <c r="G3" s="18"/>
+      <c r="I3" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="J3" s="13"/>
-      <c r="K3" s="13" t="s">
+      <c r="J3" s="17"/>
+      <c r="K3" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="L3" s="13"/>
-      <c r="M3" s="13" t="s">
+      <c r="L3" s="17"/>
+      <c r="M3" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="N3" s="14"/>
-      <c r="P3" s="12" t="s">
+      <c r="N3" s="18"/>
+      <c r="P3" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="Q3" s="13"/>
-      <c r="R3" s="13" t="s">
+      <c r="Q3" s="17"/>
+      <c r="R3" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="S3" s="13"/>
-      <c r="T3" s="13" t="s">
+      <c r="S3" s="17"/>
+      <c r="T3" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="U3" s="14"/>
-      <c r="W3" s="12" t="s">
+      <c r="U3" s="18"/>
+      <c r="W3" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="X3" s="13"/>
-      <c r="Y3" s="13" t="s">
+      <c r="X3" s="17"/>
+      <c r="Y3" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="Z3" s="13"/>
-      <c r="AA3" s="13" t="s">
+      <c r="Z3" s="17"/>
+      <c r="AA3" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="AB3" s="14"/>
-      <c r="AD3" s="12" t="s">
+      <c r="AB3" s="18"/>
+      <c r="AD3" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="AE3" s="13"/>
-      <c r="AF3" s="13" t="s">
+      <c r="AE3" s="17"/>
+      <c r="AF3" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="AG3" s="13"/>
-      <c r="AH3" s="13" t="s">
+      <c r="AG3" s="17"/>
+      <c r="AH3" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="AI3" s="14"/>
-      <c r="AK3" s="12" t="s">
+      <c r="AI3" s="18"/>
+      <c r="AK3" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="AL3" s="13"/>
-      <c r="AM3" s="13" t="s">
+      <c r="AL3" s="17"/>
+      <c r="AM3" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="AN3" s="13"/>
-      <c r="AO3" s="13" t="s">
+      <c r="AN3" s="17"/>
+      <c r="AO3" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="AP3" s="14"/>
+      <c r="AP3" s="18"/>
       <c r="AQ3" s="6"/>
     </row>
     <row r="4" spans="2:43" x14ac:dyDescent="0.2">
-      <c r="B4" s="15" t="s">
+      <c r="B4" s="12" t="s">
         <v>9</v>
       </c>
       <c r="C4">
         <v>0.16047042666438899</v>
       </c>
-      <c r="D4" s="15" t="s">
+      <c r="D4" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="E4" s="16">
+      <c r="E4" s="13">
         <v>0.108451002634894</v>
       </c>
       <c r="F4" s="1" t="s">
@@ -9145,10 +9841,10 @@
       <c r="J4">
         <v>0.16658057025509901</v>
       </c>
-      <c r="K4" s="15" t="s">
+      <c r="K4" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="L4" s="16">
+      <c r="L4" s="13">
         <v>8.5136053784184207E-2</v>
       </c>
       <c r="M4" s="1" t="s">
@@ -16756,15 +17452,11 @@
     </row>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="AM3:AN3"/>
-    <mergeCell ref="AO3:AP3"/>
-    <mergeCell ref="AD3:AE3"/>
-    <mergeCell ref="W3:X3"/>
-    <mergeCell ref="Y3:Z3"/>
-    <mergeCell ref="AA3:AB3"/>
-    <mergeCell ref="AF3:AG3"/>
-    <mergeCell ref="AH3:AI3"/>
-    <mergeCell ref="AK3:AL3"/>
+    <mergeCell ref="AK2:AP2"/>
+    <mergeCell ref="B2:G2"/>
+    <mergeCell ref="I2:N2"/>
+    <mergeCell ref="P2:U2"/>
+    <mergeCell ref="W2:AB2"/>
     <mergeCell ref="AD2:AI2"/>
     <mergeCell ref="B3:C3"/>
     <mergeCell ref="D3:E3"/>
@@ -16775,11 +17467,15 @@
     <mergeCell ref="P3:Q3"/>
     <mergeCell ref="R3:S3"/>
     <mergeCell ref="T3:U3"/>
-    <mergeCell ref="AK2:AP2"/>
-    <mergeCell ref="B2:G2"/>
-    <mergeCell ref="I2:N2"/>
-    <mergeCell ref="P2:U2"/>
-    <mergeCell ref="W2:AB2"/>
+    <mergeCell ref="AM3:AN3"/>
+    <mergeCell ref="AO3:AP3"/>
+    <mergeCell ref="AD3:AE3"/>
+    <mergeCell ref="W3:X3"/>
+    <mergeCell ref="Y3:Z3"/>
+    <mergeCell ref="AA3:AB3"/>
+    <mergeCell ref="AF3:AG3"/>
+    <mergeCell ref="AH3:AI3"/>
+    <mergeCell ref="AK3:AL3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>